<commit_message>
Add date and move text lower
</commit_message>
<xml_diff>
--- a/articles/article7/article_sheet.xlsx
+++ b/articles/article7/article_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamariorankins/repos/article_study/articles/article7/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F38A746B-8F5B-E941-9EA5-B0B0360EE598}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3006970-AF4A-F242-BDF1-D727A4D49133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -423,7 +423,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -513,7 +513,7 @@
         <v>6</v>
       </c>
       <c r="D5">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="E5" t="s">
         <v>18</v>
@@ -530,7 +530,7 @@
         <v>6</v>
       </c>
       <c r="D6">
-        <v>700</v>
+        <v>300</v>
       </c>
       <c r="E6" t="s">
         <v>19</v>

</xml_diff>